<commit_message>
adds dependencies working code in dependencies folder
</commit_message>
<xml_diff>
--- a/testing_1.xlsx
+++ b/testing_1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Parent</t>
   </si>
@@ -22,43 +22,19 @@
     <t>Methods/Children</t>
   </si>
   <si>
-    <t>ABC</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>DEF</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>add</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>sub</t>
-  </si>
-  <si>
-    <t>g</t>
+    <t>Aviral</t>
+  </si>
+  <si>
+    <t>Gauri</t>
+  </si>
+  <si>
+    <t>go_to_newyork</t>
+  </si>
+  <si>
+    <t>gauri_in_new_york</t>
+  </si>
+  <si>
+    <t>available_in_new_york</t>
   </si>
 </sst>
 </file>
@@ -416,7 +392,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -437,117 +413,22 @@
     </row>
     <row r="3" spans="1:2">
       <c r="B3" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="B4" t="s">
-        <v>4</v>
+      <c r="A4" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="B5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="B15" t="s">
+      <c r="B6" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="B17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="B19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="B21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="B22" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="B24" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>